<commit_message>
Irregular data vis basic
</commit_message>
<xml_diff>
--- a/data/t34_2000-2019.xlsx
+++ b/data/t34_2000-2019.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D1A062-4D87-457A-BC06-572DBBF7706E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A63B61A-A4F5-1443-9194-41E5D8211487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{877AD389-CC83-4D07-995B-3EB921389FC0}"/>
+    <workbookView xWindow="7780" yWindow="3600" windowWidth="23260" windowHeight="12580" xr2:uid="{877AD389-CC83-4D07-995B-3EB921389FC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 34D " sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Panama</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Global Total</t>
-  </si>
-  <si>
-    <t>2000-2009: Deportable Aliens located by Region and Country of Nationality:</t>
   </si>
 </sst>
 </file>
@@ -691,19 +688,19 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="H17" sqref="H17"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
-    <col min="2" max="10" width="10.109375" style="1" customWidth="1"/>
-    <col min="11" max="14" width="9.109375" style="1"/>
-    <col min="16" max="16" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="10" width="10.1640625" style="1" customWidth="1"/>
+    <col min="11" max="14" width="9.1640625" style="1"/>
+    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -768,7 +765,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -833,7 +830,7 @@
         <v>1013539</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -898,7 +895,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -963,7 +960,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1028,7 +1025,7 @@
         <v>99750</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1093,7 +1090,7 @@
         <v>285067</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1158,7 +1155,7 @@
         <v>268992</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1223,7 +1220,7 @@
         <v>254595</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1288,7 +1285,7 @@
         <v>14248</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -1353,7 +1350,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1368,7 +1365,7 @@
       <c r="O11"/>
       <c r="R11"/>
     </row>
-    <row r="12" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -1385,11 +1382,9 @@
       <c r="R12"/>
       <c r="U12" s="27"/>
     </row>
-    <row r="13" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13"/>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
+      <c r="B13"/>
       <c r="C13"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1403,75 +1398,75 @@
       <c r="Q13"/>
       <c r="R13"/>
     </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
       <c r="R15"/>
     </row>
-    <row r="16" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>
     </row>
-    <row r="17" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O17"/>
       <c r="P17"/>
       <c r="Q17"/>
       <c r="R17"/>
     </row>
-    <row r="18" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O18"/>
       <c r="P18"/>
       <c r="Q18"/>
       <c r="R18"/>
     </row>
-    <row r="19" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="O19"/>
       <c r="P19"/>
       <c r="Q19"/>
       <c r="R19"/>
     </row>
-    <row r="20" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="O20"/>
       <c r="P20"/>
       <c r="Q20"/>
       <c r="R20"/>
     </row>
-    <row r="21" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="O21"/>
       <c r="P21"/>
       <c r="Q21"/>
       <c r="R21"/>
     </row>
-    <row r="22" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="O22"/>
       <c r="P22"/>
       <c r="Q22"/>
       <c r="R22"/>
     </row>
-    <row r="23" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="O23"/>
       <c r="P23"/>
       <c r="Q23"/>
       <c r="R23"/>
     </row>
-    <row r="24" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="O24"/>
       <c r="P24"/>

</xml_diff>

<commit_message>
fix t34 and 41 with accurate 2009 data, add new enf graph
</commit_message>
<xml_diff>
--- a/data/t34_2000-2019.xlsx
+++ b/data/t34_2000-2019.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A63B61A-A4F5-1443-9194-41E5D8211487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EB3F69-AC05-47AA-A847-9E651F50F029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="3600" windowWidth="23260" windowHeight="12580" xr2:uid="{877AD389-CC83-4D07-995B-3EB921389FC0}"/>
+    <workbookView xWindow="11880" yWindow="2115" windowWidth="17265" windowHeight="11385" xr2:uid="{877AD389-CC83-4D07-995B-3EB921389FC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 34D " sheetId="2" r:id="rId1"/>
@@ -67,7 +67,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +95,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -178,7 +183,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -196,33 +201,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="41" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -360,6 +338,27 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -686,21 +685,21 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+      <selection pane="topRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
-    <col min="2" max="10" width="10.1640625" style="1" customWidth="1"/>
-    <col min="11" max="14" width="9.1640625" style="1"/>
-    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="2" max="10" width="10.140625" style="1" customWidth="1"/>
+    <col min="11" max="14" width="9.140625" style="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -765,39 +764,39 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="57">
+      <c r="B2" s="48">
         <v>1814729</v>
       </c>
-      <c r="C2" s="64">
+      <c r="C2" s="55">
         <v>1387486</v>
       </c>
-      <c r="D2" s="61">
+      <c r="D2" s="52">
         <v>1062279</v>
       </c>
-      <c r="E2" s="56">
+      <c r="E2" s="47">
         <v>1046422</v>
       </c>
-      <c r="F2" s="55">
+      <c r="F2" s="46">
         <v>1241089</v>
       </c>
-      <c r="G2" s="46">
+      <c r="G2" s="37">
         <v>1291142</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="28">
         <v>1206457</v>
       </c>
-      <c r="I2" s="28">
+      <c r="I2" s="19">
         <v>960756</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="9">
         <v>791575</v>
       </c>
-      <c r="K2" s="9">
-        <v>580107</v>
+      <c r="K2" s="63">
+        <v>613003</v>
       </c>
       <c r="L2" s="3">
         <v>796587</v>
@@ -830,39 +829,39 @@
         <v>1013539</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="68">
+      <c r="B3" s="59">
         <v>179</v>
       </c>
-      <c r="C3" s="65">
+      <c r="C3" s="56">
         <v>174</v>
       </c>
-      <c r="D3" s="62">
+      <c r="D3" s="53">
         <v>160</v>
       </c>
-      <c r="E3" s="58">
+      <c r="E3" s="49">
         <v>281</v>
       </c>
       <c r="F3">
         <v>151</v>
       </c>
-      <c r="G3" s="47">
+      <c r="G3" s="38">
         <v>149</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="29">
         <v>140</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3" s="20">
         <v>113</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="10">
         <v>115</v>
       </c>
-      <c r="K3" s="10">
-        <v>63</v>
+      <c r="K3">
+        <v>98</v>
       </c>
       <c r="L3" s="3">
         <v>338</v>
@@ -895,39 +894,39 @@
         <v>289</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="68">
+      <c r="B4" s="59">
         <v>328</v>
       </c>
-      <c r="C4" s="65">
+      <c r="C4" s="56">
         <v>352</v>
       </c>
-      <c r="D4" s="62">
+      <c r="D4" s="53">
         <v>334</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="49">
         <v>481</v>
       </c>
       <c r="F4">
         <v>571</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="39">
         <v>1321</v>
       </c>
-      <c r="H4" s="39">
+      <c r="H4" s="30">
         <v>803</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="21">
         <v>377</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="11">
         <v>322</v>
       </c>
-      <c r="K4" s="11">
-        <v>152</v>
+      <c r="K4">
+        <v>267</v>
       </c>
       <c r="L4" s="3">
         <v>548</v>
@@ -960,39 +959,39 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="69">
+      <c r="B5" s="60">
         <v>11845</v>
       </c>
-      <c r="C5" s="66">
+      <c r="C5" s="57">
         <v>11688</v>
       </c>
-      <c r="D5" s="62">
+      <c r="D5" s="53">
         <v>9209</v>
       </c>
-      <c r="E5" s="59">
+      <c r="E5" s="50">
         <v>11757</v>
       </c>
-      <c r="F5" s="55">
+      <c r="F5" s="46">
         <v>19180</v>
       </c>
-      <c r="G5" s="49">
+      <c r="G5" s="40">
         <v>42884</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="31">
         <v>46329</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="22">
         <v>19699</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="12">
         <v>17899</v>
       </c>
-      <c r="K5" s="12">
-        <v>956</v>
+      <c r="K5" s="64">
+        <v>16814</v>
       </c>
       <c r="L5" s="3">
         <v>29911</v>
@@ -1025,39 +1024,39 @@
         <v>99750</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="69">
+      <c r="B6" s="60">
         <v>7748</v>
       </c>
-      <c r="C6" s="66">
+      <c r="C6" s="57">
         <v>7434</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="53">
         <v>8344</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="50">
         <v>10355</v>
       </c>
-      <c r="F6" s="55">
+      <c r="F6" s="46">
         <v>14288</v>
       </c>
-      <c r="G6" s="50">
+      <c r="G6" s="41">
         <v>25908</v>
       </c>
-      <c r="H6" s="41">
+      <c r="H6" s="32">
         <v>25135</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="23">
         <v>23907</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="13">
         <v>22660</v>
       </c>
-      <c r="K6" s="13">
-        <v>1718</v>
+      <c r="K6" s="65">
+        <v>20746</v>
       </c>
       <c r="L6" s="3">
         <v>39050</v>
@@ -1090,39 +1089,39 @@
         <v>285067</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="69">
+      <c r="B7" s="60">
         <v>12075</v>
       </c>
-      <c r="C7" s="66">
+      <c r="C7" s="57">
         <v>10803</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="53">
         <v>11295</v>
       </c>
-      <c r="E7" s="59">
+      <c r="E7" s="50">
         <v>16632</v>
       </c>
-      <c r="F7" s="55">
+      <c r="F7" s="46">
         <v>26555</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="42">
         <v>55775</v>
       </c>
-      <c r="H7" s="42">
+      <c r="H7" s="33">
         <v>33365</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="24">
         <v>28263</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="14">
         <v>23785</v>
       </c>
-      <c r="K7" s="14">
-        <v>1298</v>
+      <c r="K7" s="66">
+        <v>19149</v>
       </c>
       <c r="L7" s="3">
         <v>32501</v>
@@ -1155,39 +1154,39 @@
         <v>268992</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70">
+      <c r="B8" s="61">
         <v>1744304</v>
       </c>
-      <c r="C8" s="67">
+      <c r="C8" s="58">
         <v>1315678</v>
       </c>
-      <c r="D8" s="63">
+      <c r="D8" s="54">
         <v>994724</v>
       </c>
-      <c r="E8" s="60">
+      <c r="E8" s="51">
         <v>956963</v>
       </c>
       <c r="F8" s="8">
         <v>1142807</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="43">
         <v>1093382</v>
       </c>
-      <c r="H8" s="43">
+      <c r="H8" s="34">
         <v>1057253</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="25">
         <v>854261</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="15">
         <v>693795</v>
       </c>
-      <c r="K8" s="15">
-        <v>465205</v>
+      <c r="K8" s="62">
+        <v>528139</v>
       </c>
       <c r="L8" s="3">
         <v>632034</v>
@@ -1220,39 +1219,39 @@
         <v>254595</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="69">
+      <c r="B9" s="60">
         <v>1005</v>
       </c>
-      <c r="C9" s="65">
+      <c r="C9" s="56">
         <v>990</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="53">
         <v>823</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="50">
         <v>1055</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="46">
         <v>1664</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="44">
         <v>4273</v>
       </c>
-      <c r="H9" s="44">
+      <c r="H9" s="35">
         <v>3228</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="26">
         <v>2118</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="16">
         <v>1862</v>
       </c>
-      <c r="K9" s="16">
-        <v>167</v>
+      <c r="K9" s="67">
+        <v>1478</v>
       </c>
       <c r="L9" s="3">
         <v>2587</v>
@@ -1285,39 +1284,39 @@
         <v>14248</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="68">
+      <c r="B10" s="59">
         <v>134</v>
       </c>
-      <c r="C10" s="65">
+      <c r="C10" s="56">
         <v>143</v>
       </c>
-      <c r="D10" s="62">
+      <c r="D10" s="53">
         <v>123</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="49">
         <v>126</v>
       </c>
       <c r="F10">
         <v>97</v>
       </c>
-      <c r="G10" s="54">
+      <c r="G10" s="45">
         <v>131</v>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="36">
         <v>131</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="27">
         <v>112</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="17">
         <v>135</v>
       </c>
-      <c r="K10" s="17">
-        <v>116</v>
+      <c r="K10" s="68">
+        <v>80</v>
       </c>
       <c r="L10" s="3">
         <v>283</v>
@@ -1350,7 +1349,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1365,7 +1364,7 @@
       <c r="O11"/>
       <c r="R11"/>
     </row>
-    <row r="12" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -1380,9 +1379,9 @@
       <c r="P12"/>
       <c r="Q12"/>
       <c r="R12"/>
-      <c r="U12" s="27"/>
-    </row>
-    <row r="13" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U12" s="18"/>
+    </row>
+    <row r="13" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -1398,75 +1397,75 @@
       <c r="Q13"/>
       <c r="R13"/>
     </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
       <c r="R15"/>
     </row>
-    <row r="16" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>
     </row>
-    <row r="17" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O17"/>
       <c r="P17"/>
       <c r="Q17"/>
       <c r="R17"/>
     </row>
-    <row r="18" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O18"/>
       <c r="P18"/>
       <c r="Q18"/>
       <c r="R18"/>
     </row>
-    <row r="19" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="O19"/>
       <c r="P19"/>
       <c r="Q19"/>
       <c r="R19"/>
     </row>
-    <row r="20" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="O20"/>
       <c r="P20"/>
       <c r="Q20"/>
       <c r="R20"/>
     </row>
-    <row r="21" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="O21"/>
       <c r="P21"/>
       <c r="Q21"/>
       <c r="R21"/>
     </row>
-    <row r="22" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="O22"/>
       <c r="P22"/>
       <c r="Q22"/>
       <c r="R22"/>
     </row>
-    <row r="23" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="O23"/>
       <c r="P23"/>
       <c r="Q23"/>
       <c r="R23"/>
     </row>
-    <row r="24" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="O24"/>
       <c r="P24"/>

</xml_diff>